<commit_message>
no it works for multiple, testing now needed
</commit_message>
<xml_diff>
--- a/excel_data/data/Basic Consumer_Equity_Keyfigures.xlsx
+++ b/excel_data/data/Basic Consumer_Equity_Keyfigures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/midaspavia/Documents/python_projects/excel_data_script/excel_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD1C317-43B3-4C48-9085-DF42ECEE23A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65AE76D-E8DB-B54D-98FC-D66B50F49FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="27640" windowHeight="16620" firstSheet="1" activeTab="3" xr2:uid="{A8EFDF63-01B1-4D58-BAE5-78D2830B6986}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27640" windowHeight="16620" activeTab="3" xr2:uid="{A8EFDF63-01B1-4D58-BAE5-78D2830B6986}"/>
   </bookViews>
   <sheets>
     <sheet name="M2ZkODRmZDAtMGI4NC00ND" sheetId="11" state="veryHidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9959" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9968" uniqueCount="904">
   <si>
     <t>Sub-Industry</t>
   </si>
@@ -72514,8 +72514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A732CE09-D791-47CB-9D75-D7E80120759F}">
   <dimension ref="A2:Z197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -72641,7 +72641,9 @@
       <c r="A4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -72735,7 +72737,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="42">
-        <f t="shared" ref="G4:G14" si="1">R5</f>
+        <f t="shared" ref="G5:G14" si="1">R5</f>
         <v>8.5074000000000005</v>
       </c>
       <c r="H5" s="42">
@@ -73616,7 +73618,9 @@
       <c r="A17" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
@@ -76805,7 +76809,9 @@
       <c r="A61" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="C61" s="1" t="s">
         <v>6</v>
       </c>
@@ -80969,7 +80975,9 @@
       <c r="A112" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B112" s="1"/>
+      <c r="B112" s="1" t="s">
+        <v>534</v>
+      </c>
       <c r="C112" s="1" t="s">
         <v>116</v>
       </c>
@@ -81049,7 +81057,9 @@
       <c r="A113" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B113" s="1"/>
+      <c r="B113" s="1" t="s">
+        <v>536</v>
+      </c>
       <c r="C113" s="1" t="s">
         <v>116</v>
       </c>
@@ -83127,7 +83137,9 @@
       <c r="A140" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B140" s="1"/>
+      <c r="B140" s="1" t="s">
+        <v>442</v>
+      </c>
       <c r="C140" s="1" t="s">
         <v>141</v>
       </c>
@@ -83827,7 +83839,9 @@
       <c r="A150" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B150" s="1"/>
+      <c r="B150" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="C150" s="1" t="s">
         <v>149</v>
       </c>
@@ -86052,7 +86066,9 @@
       <c r="A181" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="B181" s="1"/>
+      <c r="B181" s="1" t="s">
+        <v>509</v>
+      </c>
       <c r="C181" s="1" t="s">
         <v>177</v>
       </c>
@@ -86674,7 +86690,9 @@
       <c r="A190" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B190" s="1"/>
+      <c r="B190" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="C190" s="1" t="s">
         <v>185</v>
       </c>
@@ -87217,15 +87235,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003C253559CC884F4781DCE832A8CB1D80" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="26fe4eeb414f89c99b7c2c97f3b22ef3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eb00d37f-1d19-4fa1-b301-8f3f4b367310" xmlns:ns3="1b4b421c-b62c-43b7-a7e1-127b2a74bbe1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7af0977d678a6be0e6f430e6b840b42" ns2:_="" ns3:_="">
     <xsd:import namespace="eb00d37f-1d19-4fa1-b301-8f3f4b367310"/>
@@ -87432,15 +87441,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F48E4BC-7DCC-43BC-8116-03077F0505A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B36D551-F531-40C3-AA68-AE7C7ADEB8A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -87457,4 +87467,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F48E4BC-7DCC-43BC-8116-03077F0505A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>